<commit_message>
feat: add gsi for menuplan, refactor recipe api
</commit_message>
<xml_diff>
--- a/docs/foodlr-tables.xlsx
+++ b/docs/foodlr-tables.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23127"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24326"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\work\artifacts\free23\foodlr-service\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{D1E11E19-8A61-42AD-9644-3C5B20C847F3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{78E9DE10-822F-40F6-831C-ED7CC09207F9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{1CD5352F-E8DE-4D77-96D6-A350C1609B09}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="60">
   <si>
     <t>ean1</t>
   </si>
@@ -62,9 +62,6 @@
     <t>productGroup</t>
   </si>
   <si>
-    <t>user</t>
-  </si>
-  <si>
     <t>mv</t>
   </si>
   <si>
@@ -80,27 +77,12 @@
     <t>saison</t>
   </si>
   <si>
-    <t>ingredients</t>
-  </si>
-  <si>
-    <t>instructions</t>
-  </si>
-  <si>
     <t>RecipeTable</t>
   </si>
   <si>
     <t>barcode</t>
   </si>
   <si>
-    <t>whole year</t>
-  </si>
-  <si>
-    <t>step1, step2, step3</t>
-  </si>
-  <si>
-    <t>Milk: 1l, Butter: 200g, Flour: 500g</t>
-  </si>
-  <si>
     <t>baseItem</t>
   </si>
   <si>
@@ -119,15 +101,9 @@
     <t>flour</t>
   </si>
   <si>
-    <t>1(whole year)</t>
-  </si>
-  <si>
     <t>uuid2</t>
   </si>
   <si>
-    <t>2(spring)</t>
-  </si>
-  <si>
     <t>Foodlr Table</t>
   </si>
   <si>
@@ -165,6 +141,78 @@
   </si>
   <si>
     <t>Remove by ean</t>
+  </si>
+  <si>
+    <t>name</t>
+  </si>
+  <si>
+    <t>Burger</t>
+  </si>
+  <si>
+    <t>region</t>
+  </si>
+  <si>
+    <t>eu-central</t>
+  </si>
+  <si>
+    <t>summer</t>
+  </si>
+  <si>
+    <t>butter</t>
+  </si>
+  <si>
+    <t>sugar</t>
+  </si>
+  <si>
+    <t>Ramen</t>
+  </si>
+  <si>
+    <t>Foodlr Table GSI ByRegion</t>
+  </si>
+  <si>
+    <t>Batch Insert</t>
+  </si>
+  <si>
+    <t>Batch Delete</t>
+  </si>
+  <si>
+    <t>Get All</t>
+  </si>
+  <si>
+    <t>Get by ID</t>
+  </si>
+  <si>
+    <t>Get by Region</t>
+  </si>
+  <si>
+    <t>userId</t>
+  </si>
+  <si>
+    <t>all year</t>
+  </si>
+  <si>
+    <t>spring</t>
+  </si>
+  <si>
+    <t>uuid3</t>
+  </si>
+  <si>
+    <t>uuid4</t>
+  </si>
+  <si>
+    <t>MenuPlanTable</t>
+  </si>
+  <si>
+    <t>createdAt</t>
+  </si>
+  <si>
+    <t>recipes</t>
+  </si>
+  <si>
+    <t>shoppinglist</t>
+  </si>
+  <si>
+    <t>2021-01-01T20:23:15</t>
   </si>
 </sst>
 </file>
@@ -224,14 +272,14 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -547,87 +595,107 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9953AB53-0A1D-40FC-BB20-F46E97EA949C}">
-  <dimension ref="A1:P15"/>
+  <dimension ref="A1:U17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A9" sqref="A9:B9"/>
+    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
+      <selection activeCell="T3" sqref="T3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="2" max="2" width="13.33203125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="29.77734375" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="28" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="16.6640625" customWidth="1"/>
+    <col min="9" max="9" width="21.33203125" customWidth="1"/>
+    <col min="15" max="15" width="10" customWidth="1"/>
     <col min="16" max="16" width="16.21875" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="21" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A1" s="3" t="s">
+    <row r="1" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="A1" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="B1" s="7"/>
+      <c r="C1" s="7"/>
+      <c r="D1" s="7"/>
+      <c r="E1" s="7"/>
+      <c r="F1" s="1"/>
+      <c r="H1" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="I1" s="7"/>
+      <c r="J1" s="7"/>
+      <c r="K1" s="7"/>
+      <c r="M1" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="N1" s="7"/>
+      <c r="O1" s="7"/>
+      <c r="P1" s="7"/>
+      <c r="R1" s="7" t="s">
+        <v>55</v>
+      </c>
+      <c r="S1" s="7"/>
+      <c r="T1" s="7"/>
+      <c r="U1" s="7"/>
+    </row>
+    <row r="2" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="A2" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C2" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="D2" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="E2" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="F2" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="H2" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="I2" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="J2" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="K2" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="M2" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="B1" s="3"/>
-      <c r="C1" s="3"/>
-      <c r="D1" s="3"/>
-      <c r="E1" s="3"/>
-      <c r="F1" s="1"/>
-      <c r="H1" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="I1" s="3"/>
-      <c r="J1" s="3"/>
-      <c r="K1" s="3"/>
-      <c r="M1" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="N1" s="3"/>
-      <c r="O1" s="3"/>
-      <c r="P1" s="3"/>
-    </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A2" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="B2" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="C2" s="6" t="s">
-        <v>1</v>
-      </c>
-      <c r="D2" s="6" t="s">
-        <v>2</v>
-      </c>
-      <c r="E2" s="6" t="s">
-        <v>3</v>
-      </c>
-      <c r="F2" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="H2" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="I2" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="J2" s="6" t="s">
-        <v>1</v>
-      </c>
-      <c r="K2" s="6" t="s">
-        <v>2</v>
-      </c>
-      <c r="M2" s="4" t="s">
+      <c r="N2" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="O2" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="P2" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="N2" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="O2" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="P2" s="6" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="R2" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="S2" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="T2" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="U2" s="5" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="3" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>0</v>
       </c>
@@ -644,14 +712,14 @@
         <v>1</v>
       </c>
       <c r="F3" t="s">
-        <v>23</v>
+        <v>17</v>
       </c>
       <c r="G3" s="2"/>
       <c r="H3" t="s">
+        <v>9</v>
+      </c>
+      <c r="I3" t="s">
         <v>5</v>
-      </c>
-      <c r="I3" t="s">
-        <v>10</v>
       </c>
       <c r="J3">
         <v>1</v>
@@ -664,16 +732,22 @@
         <v>6</v>
       </c>
       <c r="N3" t="s">
-        <v>19</v>
+        <v>37</v>
       </c>
       <c r="O3" t="s">
-        <v>21</v>
+        <v>39</v>
       </c>
       <c r="P3" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.3">
+        <v>40</v>
+      </c>
+      <c r="R3" t="s">
+        <v>9</v>
+      </c>
+      <c r="S3" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="4" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>7</v>
       </c>
@@ -690,139 +764,263 @@
         <v>1</v>
       </c>
       <c r="F4" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="5" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="A5" s="7" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A5" s="3" t="s">
+      <c r="B5" s="7"/>
+      <c r="H5" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="I5" s="7"/>
+      <c r="M5" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="N5" s="7"/>
+      <c r="R5" s="7"/>
+      <c r="S5" s="7"/>
+    </row>
+    <row r="6" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="A6" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="B6" s="6"/>
+      <c r="H6" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="I6" s="6"/>
+      <c r="M6" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="N6" s="6"/>
+    </row>
+    <row r="7" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="A7" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="B7" s="6"/>
+      <c r="H7" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="I7" s="6"/>
+      <c r="M7" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="N7" s="6"/>
+    </row>
+    <row r="8" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="A8" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="B8" s="6"/>
+      <c r="E8" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="F8" s="7"/>
+      <c r="H8" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="I8" s="6"/>
+      <c r="J8" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="K8" s="7"/>
+      <c r="M8" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="B5" s="3"/>
-      <c r="H5" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="I5" s="3"/>
-      <c r="M5" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="N5" s="3"/>
-    </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A6" s="7" t="s">
-        <v>33</v>
-      </c>
-      <c r="B6" s="7"/>
-      <c r="H6" s="7" t="s">
+      <c r="N8" s="6"/>
+      <c r="O8" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="P8" s="7"/>
+    </row>
+    <row r="9" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="A9" s="6" t="s">
         <v>34</v>
       </c>
-      <c r="I6" s="7"/>
-      <c r="M6" s="7" t="s">
-        <v>38</v>
-      </c>
-      <c r="N6" s="7"/>
-    </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A7" s="7" t="s">
-        <v>41</v>
-      </c>
-      <c r="B7" s="7"/>
-      <c r="H7" s="7" t="s">
-        <v>35</v>
-      </c>
-      <c r="I7" s="7"/>
-      <c r="M7" s="7" t="s">
-        <v>39</v>
-      </c>
-      <c r="N7" s="7"/>
-    </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A8" s="7" t="s">
-        <v>43</v>
-      </c>
-      <c r="B8" s="7"/>
-      <c r="E8" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="F8" s="3"/>
-      <c r="H8" s="7" t="s">
-        <v>36</v>
-      </c>
-      <c r="I8" s="7"/>
-      <c r="M8" s="7" t="s">
-        <v>40</v>
-      </c>
-      <c r="N8" s="7"/>
-    </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A9" s="7" t="s">
-        <v>42</v>
-      </c>
-      <c r="B9" s="7"/>
-      <c r="E9" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="F9" s="5" t="s">
-        <v>26</v>
-      </c>
-      <c r="H9" s="7" t="s">
-        <v>37</v>
-      </c>
-      <c r="I9" s="7"/>
-      <c r="M9" s="7"/>
-      <c r="N9" s="7"/>
-    </row>
-    <row r="10" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="B9" s="6"/>
+      <c r="E9" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="F9" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="H9" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="I9" s="6"/>
+      <c r="J9" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="K9" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="M9" s="6" t="s">
+        <v>45</v>
+      </c>
+      <c r="N9" s="6"/>
+      <c r="O9" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="P9" s="4" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="10" spans="1:21" x14ac:dyDescent="0.3">
       <c r="E10" t="s">
         <v>0</v>
       </c>
       <c r="F10" t="s">
         <v>5</v>
       </c>
-      <c r="M10" s="7"/>
-      <c r="N10" s="7"/>
-    </row>
-    <row r="11" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="J10" t="s">
+        <v>9</v>
+      </c>
+      <c r="K10" t="s">
+        <v>5</v>
+      </c>
+      <c r="M10" s="6" t="s">
+        <v>46</v>
+      </c>
+      <c r="N10" s="6"/>
+      <c r="O10" t="s">
+        <v>6</v>
+      </c>
+      <c r="P10" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="11" spans="1:21" x14ac:dyDescent="0.3">
       <c r="E11" t="s">
         <v>7</v>
       </c>
       <c r="F11" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="12" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="J11" t="s">
+        <v>9</v>
+      </c>
+      <c r="K11" t="s">
+        <v>21</v>
+      </c>
+      <c r="M11" s="6" t="s">
+        <v>47</v>
+      </c>
+      <c r="N11" s="6"/>
+      <c r="O11" t="s">
+        <v>22</v>
+      </c>
+      <c r="P11" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="12" spans="1:21" x14ac:dyDescent="0.3">
       <c r="E12" t="s">
+        <v>9</v>
+      </c>
+      <c r="F12" t="s">
         <v>5</v>
       </c>
-      <c r="F12" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="13" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="J12" t="s">
+        <v>9</v>
+      </c>
+      <c r="K12" t="s">
+        <v>41</v>
+      </c>
+      <c r="M12" s="6" t="s">
+        <v>48</v>
+      </c>
+      <c r="N12" s="6"/>
+    </row>
+    <row r="13" spans="1:21" x14ac:dyDescent="0.3">
       <c r="E13" t="s">
-        <v>27</v>
+        <v>9</v>
       </c>
       <c r="F13" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="14" spans="1:16" x14ac:dyDescent="0.3">
+        <v>21</v>
+      </c>
+      <c r="J13" t="s">
+        <v>9</v>
+      </c>
+      <c r="K13" t="s">
+        <v>42</v>
+      </c>
+      <c r="M13" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="N13" s="6"/>
+    </row>
+    <row r="14" spans="1:21" x14ac:dyDescent="0.3">
       <c r="E14" t="s">
         <v>6</v>
       </c>
       <c r="F14" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="15" spans="1:16" x14ac:dyDescent="0.3">
+        <v>51</v>
+      </c>
+      <c r="O14" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="P14" s="7"/>
+    </row>
+    <row r="15" spans="1:21" x14ac:dyDescent="0.3">
       <c r="E15" t="s">
-        <v>29</v>
+        <v>22</v>
       </c>
       <c r="F15" t="s">
-        <v>30</v>
+        <v>52</v>
+      </c>
+      <c r="O15" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="P15" s="4" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="16" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="E16" t="s">
+        <v>53</v>
+      </c>
+      <c r="F16" t="s">
+        <v>37</v>
+      </c>
+      <c r="O16" t="s">
+        <v>39</v>
+      </c>
+      <c r="P16" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="17" spans="5:6" x14ac:dyDescent="0.3">
+      <c r="E17" t="s">
+        <v>54</v>
+      </c>
+      <c r="F17" t="s">
+        <v>43</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="20">
+  <mergeCells count="28">
+    <mergeCell ref="R1:U1"/>
+    <mergeCell ref="R5:S5"/>
+    <mergeCell ref="J8:K8"/>
+    <mergeCell ref="O8:P8"/>
+    <mergeCell ref="O14:P14"/>
+    <mergeCell ref="M11:N11"/>
+    <mergeCell ref="M12:N12"/>
+    <mergeCell ref="M13:N13"/>
+    <mergeCell ref="A1:E1"/>
+    <mergeCell ref="H1:K1"/>
+    <mergeCell ref="M1:P1"/>
+    <mergeCell ref="E8:F8"/>
+    <mergeCell ref="A5:B5"/>
+    <mergeCell ref="H5:I5"/>
+    <mergeCell ref="M5:N5"/>
+    <mergeCell ref="H6:I6"/>
+    <mergeCell ref="H7:I7"/>
+    <mergeCell ref="H8:I8"/>
     <mergeCell ref="M10:N10"/>
     <mergeCell ref="A6:B6"/>
     <mergeCell ref="A7:B7"/>
@@ -833,16 +1031,6 @@
     <mergeCell ref="M7:N7"/>
     <mergeCell ref="M8:N8"/>
     <mergeCell ref="M9:N9"/>
-    <mergeCell ref="A1:E1"/>
-    <mergeCell ref="H1:K1"/>
-    <mergeCell ref="M1:P1"/>
-    <mergeCell ref="E8:F8"/>
-    <mergeCell ref="A5:B5"/>
-    <mergeCell ref="H5:I5"/>
-    <mergeCell ref="M5:N5"/>
-    <mergeCell ref="H6:I6"/>
-    <mergeCell ref="H7:I7"/>
-    <mergeCell ref="H8:I8"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>